<commit_message>
In Text some functions added
</commit_message>
<xml_diff>
--- a/🟡 Intermediate Level (Analysis Tools)/🧮 Chapter 5 - Core Formulas & Functions/Text/Left_function.xlsx
+++ b/🟡 Intermediate Level (Analysis Tools)/🧮 Chapter 5 - Core Formulas & Functions/Text/Left_function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Science\Self Learning\Excel\🟡 Intermediate Level (Analysis Tools)\🧮 Chapter 5 - Core Formulas &amp; Functions\Text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA7EEA6-63D7-4A67-8494-86FEA6D17C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE984C69-B369-4758-894B-5B4BAD523A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>